<commit_message>
fixed column name in wages table
</commit_message>
<xml_diff>
--- a/dissdata/data/LabourMarket/econ_labour_wages_tbl_METADATA.xlsx
+++ b/dissdata/data/LabourMarket/econ_labour_wages_tbl_METADATA.xlsx
@@ -174,9 +174,6 @@
     <t>nechako_annual_wage</t>
   </si>
   <si>
-    <t>ne_coast_low_wage</t>
-  </si>
-  <si>
     <t>ne_median_wage</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>ne_low_wage</t>
   </si>
 </sst>
 </file>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -580,13 +580,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -846,32 +846,32 @@
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>